<commit_message>
sorted out EOS mess, adding inversion of T for P and rho
</commit_message>
<xml_diff>
--- a/docs/Examples/Example7_Useful_EOS_Calcs/Batch_processing_TC.xlsx
+++ b/docs/Examples/Example7_Useful_EOS_Calcs/Batch_processing_TC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Berkeley_NEW\DiadFit_outer\docs\Examples\Example7_Useful_EOS_Calcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13C427F-7DBB-4864-B17B-336528101DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{928D4A5F-B84E-4B18-ABC3-750D9C77525A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15960" xr2:uid="{9022BC05-3138-46E6-A3AD-C82E9882530C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9022BC05-3138-46E6-A3AD-C82E9882530C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -453,7 +453,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -513,7 +513,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>